<commit_message>
commit 20 - menambahkan positive test case checkout
</commit_message>
<xml_diff>
--- a/Data Files/alldataproject.xlsx
+++ b/Data Files/alldataproject.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\git\Final-Project-QA-WEB\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62BAABA-C039-4FB0-B895-FD14C1C9A115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF19DF3-04E5-476A-A52C-4F8361B05C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CDC13DA7-A7AE-469B-B975-05DDD0C89D22}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CDC13DA7-A7AE-469B-B975-05DDD0C89D22}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
     <sheet name="Register" sheetId="1" r:id="rId2"/>
     <sheet name="Filter" sheetId="3" r:id="rId3"/>
+    <sheet name="data laptop" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>username</t>
   </si>
@@ -131,6 +132,18 @@
   </si>
   <si>
     <t>COMPATIBILITY</t>
+  </si>
+  <si>
+    <t>datalaptop</t>
+  </si>
+  <si>
+    <t>LAPTOP A</t>
+  </si>
+  <si>
+    <t>LAPTOP B</t>
+  </si>
+  <si>
+    <t>KOMPUTER</t>
   </si>
 </sst>
 </file>
@@ -704,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5967C586-81E7-47CD-A788-F919B3238369}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -741,4 +754,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50208B8E-7F65-4A73-9421-3834B289D2F5}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commit 24 - menambahkan assertion pada test case
</commit_message>
<xml_diff>
--- a/Data Files/alldataproject.xlsx
+++ b/Data Files/alldataproject.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\git\Final-Project-QA-WEB\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF19DF3-04E5-476A-A52C-4F8361B05C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8159DC-1810-4FF3-A15C-176BDD867396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CDC13DA7-A7AE-469B-B975-05DDD0C89D22}"/>
+    <workbookView xWindow="3132" yWindow="3168" windowWidth="17280" windowHeight="9072" activeTab="4" xr2:uid="{CDC13DA7-A7AE-469B-B975-05DDD0C89D22}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
     <sheet name="Register" sheetId="1" r:id="rId2"/>
     <sheet name="Filter" sheetId="3" r:id="rId3"/>
     <sheet name="data laptop" sheetId="4" r:id="rId4"/>
+    <sheet name="data contact us" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>username</t>
   </si>
@@ -144,6 +145,18 @@
   </si>
   <si>
     <t>KOMPUTER</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>yudhatesting@gmail.com</t>
+  </si>
+  <si>
+    <t>this product so cool!</t>
+  </si>
+  <si>
+    <t>I want to buy this product</t>
   </si>
 </sst>
 </file>
@@ -760,7 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50208B8E-7F65-4A73-9421-3834B289D2F5}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -792,4 +805,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905D1AC3-8F9D-4AF7-A9F4-E1E771D9D800}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{66B7861A-B53C-4C29-9830-4521DD06E0AF}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{DD1DEF0B-5C5F-493C-8D32-623A471D7BAF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commit 26 - pembuatan all test suite
</commit_message>
<xml_diff>
--- a/Data Files/alldataproject.xlsx
+++ b/Data Files/alldataproject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\git\Final-Project-QA-WEB\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8159DC-1810-4FF3-A15C-176BDD867396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFC0EEA-ED2B-4ECF-9DBF-160506732585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3132" yWindow="3168" windowWidth="17280" windowHeight="9072" activeTab="4" xr2:uid="{CDC13DA7-A7AE-469B-B975-05DDD0C89D22}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{CDC13DA7-A7AE-469B-B975-05DDD0C89D22}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Filter" sheetId="3" r:id="rId3"/>
     <sheet name="data laptop" sheetId="4" r:id="rId4"/>
     <sheet name="data contact us" sheetId="5" r:id="rId5"/>
+    <sheet name="checkout safepay" sheetId="6" r:id="rId6"/>
+    <sheet name="checkout wihout login" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>username</t>
   </si>
@@ -163,7 +165,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +177,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -585,7 +593,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,7 +819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905D1AC3-8F9D-4AF7-A9F4-E1E771D9D800}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -852,4 +860,91 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2EE1C82-6EF9-4C52-8C26-654B82EDCED3}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17948E4E-F156-49CC-8C30-A54DBDFBE383}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commit 28 - penambahan test suite collection dan scenario negative test case
</commit_message>
<xml_diff>
--- a/Data Files/alldataproject.xlsx
+++ b/Data Files/alldataproject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\git\Final-Project-QA-WEB\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFC0EEA-ED2B-4ECF-9DBF-160506732585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2834A9FD-3EB1-4821-9624-898F2B250C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{CDC13DA7-A7AE-469B-B975-05DDD0C89D22}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="9" xr2:uid="{CDC13DA7-A7AE-469B-B975-05DDD0C89D22}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,10 @@
     <sheet name="data contact us" sheetId="5" r:id="rId5"/>
     <sheet name="checkout safepay" sheetId="6" r:id="rId6"/>
     <sheet name="checkout wihout login" sheetId="7" r:id="rId7"/>
+    <sheet name="login negative test case" sheetId="8" r:id="rId8"/>
+    <sheet name="data gagal checkout" sheetId="9" r:id="rId9"/>
+    <sheet name="data contact us gagal" sheetId="10" r:id="rId10"/>
+    <sheet name="data keyword" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
   <si>
     <t>username</t>
   </si>
@@ -146,9 +150,6 @@
     <t>LAPTOP B</t>
   </si>
   <si>
-    <t>KOMPUTER</t>
-  </si>
-  <si>
     <t>subject</t>
   </si>
   <si>
@@ -159,6 +160,18 @@
   </si>
   <si>
     <t>I want to buy this product</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>naruto</t>
+  </si>
+  <si>
+    <t>one piece</t>
+  </si>
+  <si>
+    <t>bleach</t>
   </si>
 </sst>
 </file>
@@ -550,7 +563,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,12 +601,94 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{425AB301-62AC-415D-9D03-F3A7083B06CB}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="yudhatesting@gmail.com" xr:uid="{5356D3ED-8A3B-4746-A41A-E12A8948BC3C}"/>
+    <hyperlink ref="A3" r:id="rId2" display="yudhatesting@" xr:uid="{8AD4ACC8-B215-4320-9B74-1654618A0CB4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C12940E-1A43-4A12-AACE-F1373D207E01}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80EC329-E4D3-49A4-A1BC-0C539DCD8B6C}">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,10 +874,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50208B8E-7F65-4A73-9421-3834B289D2F5}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,11 +900,6 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -820,7 +910,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,15 +924,15 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -850,7 +940,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -867,7 +957,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17948E4E-F156-49CC-8C30-A54DBDFBE383}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,4 +1037,90 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD69555-5468-45B7-AF55-490B743C69FC}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>12345678</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82E1E85-47C4-4D9C-A139-2B4663BBF113}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>12345678</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commit 30 - testing test suite collection positive and negative case
</commit_message>
<xml_diff>
--- a/Data Files/alldataproject.xlsx
+++ b/Data Files/alldataproject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\git\Final-Project-QA-WEB\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2834A9FD-3EB1-4821-9624-898F2B250C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EF4CAB-52E7-4349-B5B8-80E7EB36BC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="9" xr2:uid="{CDC13DA7-A7AE-469B-B975-05DDD0C89D22}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="11" xr2:uid="{CDC13DA7-A7AE-469B-B975-05DDD0C89D22}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="data gagal checkout" sheetId="9" r:id="rId9"/>
     <sheet name="data contact us gagal" sheetId="10" r:id="rId10"/>
     <sheet name="data keyword" sheetId="11" r:id="rId11"/>
+    <sheet name="data address" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
   <si>
     <t>username</t>
   </si>
@@ -172,6 +173,15 @@
   </si>
   <si>
     <t>bleach</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>Jalan Medan Merdeka No 5 Jakarta</t>
+  </si>
+  <si>
+    <t>Oma Regency Mampang Jakarta</t>
   </si>
 </sst>
 </file>
@@ -605,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{425AB301-62AC-415D-9D03-F3A7083B06CB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -653,7 +663,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,6 +686,49 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721220C2-E75D-4515-8B9C-800976D5A65C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1001,7 +1054,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>